<commit_message>
Updating BPoEFUbVT, BVsTL, PVsTL for LCFS updates for FF55
</commit_message>
<xml_diff>
--- a/InputData/trans/BVTStL/Boolean Veh Types Subject to LCFS.xlsx
+++ b/InputData/trans/BVTStL/Boolean Veh Types Subject to LCFS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\trans\BVTStL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\Vensim files from GitHub\EPS EU\InputData\trans\BVTStL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B748A387-264B-4ED0-9400-910230BD852C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F5FFD1-2CD2-403E-979F-3EAC8617CB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="720" windowWidth="26730" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="465" yWindow="1320" windowWidth="16695" windowHeight="15135" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -442,7 +442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -524,8 +524,8 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,10 +551,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -562,10 +562,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -584,10 +584,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -595,10 +595,10 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -606,10 +606,10 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>